<commit_message>
First full draft of starting point.
</commit_message>
<xml_diff>
--- a/Proposal/figures/Example.xlsx
+++ b/Proposal/figures/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrikleopold/Documents/workspace/dfg-SemanticUILogMining/Proposal/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FD7A77-C5EF-9242-9153-B30BAD176DC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3247E99D-0302-0444-8279-0B52E9264B1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37480" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{7CE3DEE8-1F13-C144-9716-38AB606075C5}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K17"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>